<commit_message>
Changes made to accomodate compiler changes
</commit_message>
<xml_diff>
--- a/src/main/resources/FeatureFiles/ProfessionalServicePageTestCases.xlsx
+++ b/src/main/resources/FeatureFiles/ProfessionalServicePageTestCases.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gurcharan/Desktop/CouchBase/src/main/resources/FeatureFiles/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16592681-DAA6-ED40-B1B7-A90771F5ED5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -225,9 +231,6 @@
     <t>ContactPage_TextBox_Zip</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
     <t>1234567</t>
   </si>
   <si>
@@ -286,12 +289,15 @@
   </si>
   <si>
     <t>deviceConfig.browser</t>
+  </si>
+  <si>
+    <t>{null}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -368,9 +374,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -408,7 +414,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -480,7 +486,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -653,23 +659,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="C143" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="D162" sqref="D162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="91.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.453125" customWidth="1"/>
+    <col min="1" max="1" width="91.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -686,29 +692,29 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -716,7 +722,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
@@ -724,7 +730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -732,12 +738,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>54</v>
       </c>
@@ -751,7 +757,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>25</v>
       </c>
@@ -762,7 +768,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -773,7 +779,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -784,7 +790,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>6</v>
       </c>
@@ -795,7 +801,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>25</v>
       </c>
@@ -806,7 +812,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>6</v>
       </c>
@@ -817,7 +823,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>25</v>
       </c>
@@ -828,7 +834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
@@ -839,7 +845,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
@@ -850,7 +856,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
@@ -861,7 +867,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
@@ -869,7 +875,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>5</v>
       </c>
@@ -877,7 +883,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>56</v>
       </c>
@@ -891,7 +897,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>55</v>
       </c>
@@ -902,7 +908,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
@@ -913,7 +919,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
         <v>55</v>
       </c>
@@ -924,7 +930,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>6</v>
       </c>
@@ -935,7 +941,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
         <v>55</v>
       </c>
@@ -946,7 +952,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>6</v>
       </c>
@@ -957,7 +963,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
         <v>55</v>
       </c>
@@ -968,7 +974,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>13</v>
       </c>
@@ -979,7 +985,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>13</v>
       </c>
@@ -990,7 +996,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
@@ -1001,7 +1007,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
         <v>20</v>
       </c>
@@ -1009,7 +1015,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>5</v>
       </c>
@@ -1017,7 +1023,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>37</v>
       </c>
@@ -1028,7 +1034,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>62</v>
       </c>
@@ -1042,7 +1048,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>25</v>
       </c>
@@ -1053,7 +1059,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
@@ -1064,7 +1070,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>25</v>
       </c>
@@ -1075,7 +1081,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>6</v>
       </c>
@@ -1086,7 +1092,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>25</v>
       </c>
@@ -1097,7 +1103,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>6</v>
       </c>
@@ -1108,7 +1114,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>25</v>
       </c>
@@ -1119,7 +1125,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B46" s="2" t="s">
         <v>13</v>
       </c>
@@ -1130,7 +1136,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B47" s="2" t="s">
         <v>13</v>
       </c>
@@ -1141,7 +1147,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
         <v>6</v>
       </c>
@@ -1152,7 +1158,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
         <v>20</v>
       </c>
@@ -1160,7 +1166,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
         <v>5</v>
       </c>
@@ -1168,7 +1174,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
         <v>37</v>
       </c>
@@ -1179,7 +1185,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>63</v>
       </c>
@@ -1193,7 +1199,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>25</v>
       </c>
@@ -1204,7 +1210,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B55" s="2" t="s">
         <v>6</v>
       </c>
@@ -1215,7 +1221,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>25</v>
       </c>
@@ -1226,7 +1232,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B57" s="2" t="s">
         <v>6</v>
       </c>
@@ -1237,7 +1243,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>25</v>
       </c>
@@ -1248,7 +1254,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="s">
         <v>6</v>
       </c>
@@ -1259,7 +1265,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>25</v>
       </c>
@@ -1270,7 +1276,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B61" s="2" t="s">
         <v>13</v>
       </c>
@@ -1281,7 +1287,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B62" s="2" t="s">
         <v>13</v>
       </c>
@@ -1292,7 +1298,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B63" s="2" t="s">
         <v>6</v>
       </c>
@@ -1303,7 +1309,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
         <v>20</v>
       </c>
@@ -1311,7 +1317,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B65" s="2" t="s">
         <v>5</v>
       </c>
@@ -1319,7 +1325,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B66" s="2" t="s">
         <v>37</v>
       </c>
@@ -1330,7 +1336,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>57</v>
       </c>
@@ -1344,7 +1350,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>25</v>
       </c>
@@ -1355,7 +1361,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B70" s="2" t="s">
         <v>6</v>
       </c>
@@ -1366,7 +1372,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>25</v>
       </c>
@@ -1377,7 +1383,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B72" s="2" t="s">
         <v>6</v>
       </c>
@@ -1388,7 +1394,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>25</v>
       </c>
@@ -1399,7 +1405,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B74" s="2" t="s">
         <v>6</v>
       </c>
@@ -1410,7 +1416,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>25</v>
       </c>
@@ -1421,7 +1427,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B76" s="2" t="s">
         <v>13</v>
       </c>
@@ -1432,7 +1438,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B77" s="2" t="s">
         <v>13</v>
       </c>
@@ -1443,7 +1449,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B78" s="2" t="s">
         <v>6</v>
       </c>
@@ -1454,7 +1460,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B79" s="2" t="s">
         <v>20</v>
       </c>
@@ -1462,7 +1468,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B80" s="2" t="s">
         <v>5</v>
       </c>
@@ -1470,7 +1476,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B81" s="2" t="s">
         <v>37</v>
       </c>
@@ -1481,7 +1487,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>58</v>
       </c>
@@ -1495,7 +1501,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>25</v>
       </c>
@@ -1506,7 +1512,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B85" s="2" t="s">
         <v>6</v>
       </c>
@@ -1517,7 +1523,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>25</v>
       </c>
@@ -1528,7 +1534,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B87" s="2" t="s">
         <v>6</v>
       </c>
@@ -1539,7 +1545,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>25</v>
       </c>
@@ -1550,7 +1556,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B89" s="2" t="s">
         <v>6</v>
       </c>
@@ -1561,7 +1567,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>25</v>
       </c>
@@ -1572,7 +1578,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B91" s="2" t="s">
         <v>13</v>
       </c>
@@ -1583,7 +1589,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B92" s="2" t="s">
         <v>13</v>
       </c>
@@ -1594,7 +1600,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B93" s="2" t="s">
         <v>20</v>
       </c>
@@ -1602,7 +1608,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B94" s="2" t="s">
         <v>5</v>
       </c>
@@ -1610,7 +1616,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B95" s="2" t="s">
         <v>37</v>
       </c>
@@ -1621,7 +1627,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>59</v>
       </c>
@@ -1635,7 +1641,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>25</v>
       </c>
@@ -1646,7 +1652,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B99" s="2" t="s">
         <v>6</v>
       </c>
@@ -1657,7 +1663,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>25</v>
       </c>
@@ -1668,7 +1674,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B101" s="2" t="s">
         <v>6</v>
       </c>
@@ -1679,7 +1685,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>25</v>
       </c>
@@ -1690,7 +1696,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B103" s="2" t="s">
         <v>6</v>
       </c>
@@ -1701,7 +1707,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>25</v>
       </c>
@@ -1712,7 +1718,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B105" s="2" t="s">
         <v>13</v>
       </c>
@@ -1723,7 +1729,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B106" s="2" t="s">
         <v>6</v>
       </c>
@@ -1734,7 +1740,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B107" s="2" t="s">
         <v>20</v>
       </c>
@@ -1742,7 +1748,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B108" s="2" t="s">
         <v>5</v>
       </c>
@@ -1750,7 +1756,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B109" s="2" t="s">
         <v>37</v>
       </c>
@@ -1761,7 +1767,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>60</v>
       </c>
@@ -1775,7 +1781,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
         <v>25</v>
       </c>
@@ -1786,7 +1792,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B113" s="2" t="s">
         <v>6</v>
       </c>
@@ -1797,7 +1803,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>25</v>
       </c>
@@ -1808,7 +1814,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B115" s="2" t="s">
         <v>6</v>
       </c>
@@ -1819,7 +1825,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>25</v>
       </c>
@@ -1830,7 +1836,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B117" s="2" t="s">
         <v>6</v>
       </c>
@@ -1841,7 +1847,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>25</v>
       </c>
@@ -1852,7 +1858,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B119" s="2" t="s">
         <v>13</v>
       </c>
@@ -1863,7 +1869,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B120" s="2" t="s">
         <v>6</v>
       </c>
@@ -1874,7 +1880,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B121" s="2" t="s">
         <v>20</v>
       </c>
@@ -1882,7 +1888,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B122" s="2" t="s">
         <v>5</v>
       </c>
@@ -1890,7 +1896,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B123" s="2" t="s">
         <v>37</v>
       </c>
@@ -1901,9 +1907,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>6</v>
@@ -1915,7 +1921,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B126" s="2" t="s">
         <v>25</v>
       </c>
@@ -1926,7 +1932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B127" s="2" t="s">
         <v>6</v>
       </c>
@@ -1937,7 +1943,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B128" s="2" t="s">
         <v>25</v>
       </c>
@@ -1948,7 +1954,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B129" s="2" t="s">
         <v>6</v>
       </c>
@@ -1959,7 +1965,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B130" s="2" t="s">
         <v>25</v>
       </c>
@@ -1970,7 +1976,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B131" s="2" t="s">
         <v>13</v>
       </c>
@@ -1981,7 +1987,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B132" s="2" t="s">
         <v>13</v>
       </c>
@@ -1992,7 +1998,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B133" s="2" t="s">
         <v>6</v>
       </c>
@@ -2003,7 +2009,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B134" s="2" t="s">
         <v>20</v>
       </c>
@@ -2011,7 +2017,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B135" s="2" t="s">
         <v>5</v>
       </c>
@@ -2019,7 +2025,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B136" s="2" t="s">
         <v>37</v>
       </c>
@@ -2030,9 +2036,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>6</v>
@@ -2044,7 +2050,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B139" s="2" t="s">
         <v>25</v>
       </c>
@@ -2055,7 +2061,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B140" s="2" t="s">
         <v>6</v>
       </c>
@@ -2066,7 +2072,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B141" s="2" t="s">
         <v>25</v>
       </c>
@@ -2077,7 +2083,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B142" s="2" t="s">
         <v>6</v>
       </c>
@@ -2088,7 +2094,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B143" s="2" t="s">
         <v>25</v>
       </c>
@@ -2099,7 +2105,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B144" s="2" t="s">
         <v>13</v>
       </c>
@@ -2110,7 +2116,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B145" s="2" t="s">
         <v>13</v>
       </c>
@@ -2121,7 +2127,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B146" s="2" t="s">
         <v>6</v>
       </c>
@@ -2132,7 +2138,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B147" s="2" t="s">
         <v>20</v>
       </c>
@@ -2140,7 +2146,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B148" s="2" t="s">
         <v>5</v>
       </c>
@@ -2148,7 +2154,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B149" s="2" t="s">
         <v>37</v>
       </c>
@@ -2159,9 +2165,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>6</v>
@@ -2173,7 +2179,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B152" s="2" t="s">
         <v>25</v>
       </c>
@@ -2184,7 +2190,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B153" s="2" t="s">
         <v>6</v>
       </c>
@@ -2195,7 +2201,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B154" s="2" t="s">
         <v>25</v>
       </c>
@@ -2206,7 +2212,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B155" s="2" t="s">
         <v>6</v>
       </c>
@@ -2217,7 +2223,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B156" s="2" t="s">
         <v>25</v>
       </c>
@@ -2228,7 +2234,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B157" s="2" t="s">
         <v>6</v>
       </c>
@@ -2239,7 +2245,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B158" s="2" t="s">
         <v>25</v>
       </c>
@@ -2250,7 +2256,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B159" s="2" t="s">
         <v>13</v>
       </c>
@@ -2261,7 +2267,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B160" s="2" t="s">
         <v>5</v>
       </c>
@@ -2269,7 +2275,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B161" s="2" t="s">
         <v>6</v>
       </c>
@@ -2280,7 +2286,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B162" s="2" t="s">
         <v>55</v>
       </c>
@@ -2288,10 +2294,10 @@
         <v>67</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B163" s="2" t="s">
         <v>6</v>
       </c>
@@ -2299,10 +2305,10 @@
         <v>67</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B164" s="5" t="s">
         <v>55</v>
       </c>
@@ -2310,10 +2316,10 @@
         <v>67</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B165" s="2" t="s">
         <v>13</v>
       </c>
@@ -2324,7 +2330,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B166" s="2" t="s">
         <v>6</v>
       </c>
@@ -2335,7 +2341,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B167" s="2" t="s">
         <v>20</v>
       </c>
@@ -2343,7 +2349,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B168" s="2" t="s">
         <v>5</v>
       </c>
@@ -2351,9 +2357,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B170" s="2" t="s">
         <v>6</v>
@@ -2365,7 +2371,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B171" s="2" t="s">
         <v>25</v>
       </c>
@@ -2376,7 +2382,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B172" s="2" t="s">
         <v>6</v>
       </c>
@@ -2387,7 +2393,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B173" s="2" t="s">
         <v>25</v>
       </c>
@@ -2398,7 +2404,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B174" s="2" t="s">
         <v>6</v>
       </c>
@@ -2409,7 +2415,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B175" s="2" t="s">
         <v>25</v>
       </c>
@@ -2420,7 +2426,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B176" s="2" t="s">
         <v>6</v>
       </c>
@@ -2431,7 +2437,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B177" s="2" t="s">
         <v>25</v>
       </c>
@@ -2442,7 +2448,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B178" s="2" t="s">
         <v>13</v>
       </c>
@@ -2453,7 +2459,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B179" s="2" t="s">
         <v>13</v>
       </c>
@@ -2464,7 +2470,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B180" s="2" t="s">
         <v>6</v>
       </c>
@@ -2475,7 +2481,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B181" s="2" t="s">
         <v>20</v>
       </c>
@@ -2483,28 +2489,28 @@
         <v>21</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B182" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B183" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B185" s="2" t="s">
         <v>6</v>
@@ -2516,7 +2522,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B186" s="2" t="s">
         <v>25</v>
       </c>
@@ -2527,7 +2533,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B187" s="2" t="s">
         <v>6</v>
       </c>
@@ -2538,7 +2544,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B188" s="2" t="s">
         <v>25</v>
       </c>
@@ -2549,7 +2555,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B189" s="2" t="s">
         <v>6</v>
       </c>
@@ -2560,7 +2566,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B190" s="2" t="s">
         <v>25</v>
       </c>
@@ -2571,7 +2577,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B191" s="2" t="s">
         <v>6</v>
       </c>
@@ -2582,7 +2588,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B192" s="2" t="s">
         <v>25</v>
       </c>
@@ -2593,7 +2599,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B193" s="2" t="s">
         <v>13</v>
       </c>
@@ -2601,29 +2607,29 @@
         <v>14</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B194" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C194" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B195" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C195" t="s">
+        <v>72</v>
+      </c>
+      <c r="D195" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D195" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B196" s="2" t="s">
         <v>13</v>
       </c>
@@ -2634,7 +2640,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B197" s="2" t="s">
         <v>6</v>
       </c>
@@ -2645,15 +2651,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B198" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B199" s="2" t="s">
         <v>20</v>
       </c>
@@ -2661,7 +2667,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B200" s="2" t="s">
         <v>5</v>
       </c>
@@ -2669,9 +2675,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B202" s="2" t="s">
         <v>6</v>
@@ -2683,7 +2689,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B203" s="2" t="s">
         <v>25</v>
       </c>
@@ -2694,7 +2700,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B204" s="2" t="s">
         <v>6</v>
       </c>
@@ -2705,7 +2711,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B205" s="2" t="s">
         <v>25</v>
       </c>
@@ -2716,7 +2722,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B206" s="2" t="s">
         <v>6</v>
       </c>
@@ -2727,7 +2733,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B207" s="2" t="s">
         <v>25</v>
       </c>
@@ -2738,7 +2744,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B208" s="2" t="s">
         <v>6</v>
       </c>
@@ -2749,7 +2755,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B209" s="2" t="s">
         <v>25</v>
       </c>
@@ -2760,7 +2766,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B210" s="2" t="s">
         <v>13</v>
       </c>
@@ -2768,10 +2774,10 @@
         <v>14</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B211" s="2" t="s">
         <v>13</v>
       </c>
@@ -2782,7 +2788,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B212" s="2" t="s">
         <v>6</v>
       </c>
@@ -2793,7 +2799,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B213" s="2" t="s">
         <v>20</v>
       </c>
@@ -2801,28 +2807,28 @@
         <v>21</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B214" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B215" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D215" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B217" s="2" t="s">
         <v>6</v>
@@ -2834,7 +2840,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B218" s="2" t="s">
         <v>25</v>
       </c>
@@ -2845,7 +2851,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B219" s="2" t="s">
         <v>6</v>
       </c>
@@ -2856,7 +2862,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B220" s="2" t="s">
         <v>25</v>
       </c>
@@ -2867,7 +2873,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B221" s="2" t="s">
         <v>6</v>
       </c>
@@ -2878,7 +2884,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B222" s="2" t="s">
         <v>25</v>
       </c>
@@ -2889,7 +2895,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B223" s="2" t="s">
         <v>6</v>
       </c>
@@ -2900,7 +2906,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B224" s="2" t="s">
         <v>25</v>
       </c>
@@ -2911,7 +2917,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B225" s="2" t="s">
         <v>13</v>
       </c>
@@ -2919,29 +2925,29 @@
         <v>14</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B226" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C226" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B227" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C227" t="s">
+        <v>72</v>
+      </c>
+      <c r="D227" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D227" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B228" s="2" t="s">
         <v>13</v>
       </c>
@@ -2952,7 +2958,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B229" s="2" t="s">
         <v>6</v>
       </c>
@@ -2963,34 +2969,34 @@
         <v>19</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B230" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B231" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C231" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D231" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D231" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B232" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B233" s="2" t="s">
         <v>20</v>
       </c>
@@ -2998,7 +3004,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B234" s="2" t="s">
         <v>5</v>
       </c>
@@ -3006,7 +3012,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" s="2" t="s">
         <v>34</v>
       </c>
@@ -3016,7 +3022,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D57" r:id="rId1"/>
+    <hyperlink ref="D57" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -3024,18 +3030,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.6328125" style="2"/>
-    <col min="2" max="2" width="23.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.6328125" style="2"/>
+    <col min="1" max="1" width="8.6640625" style="2"/>
+    <col min="2" max="2" width="23.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -3076,12 +3082,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>